<commit_message>
This is my second build commit
</commit_message>
<xml_diff>
--- a/FileInput/DataEngine.xlsx
+++ b/FileInput/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8796" tabRatio="783" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8796" tabRatio="783"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="139">
   <si>
     <t>TCID</t>
   </si>
@@ -314,13 +314,145 @@
   </si>
   <si>
     <t>ValidateTable</t>
+  </si>
+  <si>
+    <t>Wait for supplier link</t>
+  </si>
+  <si>
+    <t>Click Supplier link</t>
+  </si>
+  <si>
+    <t>(//a[contains(.,'Suppliers')])[2]</t>
+  </si>
+  <si>
+    <t>Wait for supplir number</t>
+  </si>
+  <si>
+    <t>Capture supplier number</t>
+  </si>
+  <si>
+    <t>Enterr Address</t>
+  </si>
+  <si>
+    <t>Enter City</t>
+  </si>
+  <si>
+    <t>Enter Country</t>
+  </si>
+  <si>
+    <t>Enter ContactPerson</t>
+  </si>
+  <si>
+    <t>Enter Phone number</t>
+  </si>
+  <si>
+    <t>Enter Mobile number</t>
+  </si>
+  <si>
+    <t>Enter Email</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Supplier_Name']</t>
+  </si>
+  <si>
+    <t>//textarea[@id='x_Address']</t>
+  </si>
+  <si>
+    <t>//textarea[@id='x_Notes']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_City']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Country']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Contact_Person']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Phone_Number']</t>
+  </si>
+  <si>
+    <t>//input[@id='x__Email']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Mobile_Number']</t>
+  </si>
+  <si>
+    <t>LG Suppliers</t>
+  </si>
+  <si>
+    <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>Kukatpalli,KPHP,9th phase 243</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>QedgeTech</t>
+  </si>
+  <si>
+    <t>I am supplying LG goods</t>
+  </si>
+  <si>
+    <t>supplierTable</t>
+  </si>
+  <si>
+    <t>captureSupplier</t>
+  </si>
+  <si>
+    <t>Click Customer link</t>
+  </si>
+  <si>
+    <t>Wait for Customer link</t>
+  </si>
+  <si>
+    <t>Wait for Customer number</t>
+  </si>
+  <si>
+    <t>Capture Customer number</t>
+  </si>
+  <si>
+    <t>Enter Customer name</t>
+  </si>
+  <si>
+    <t>Enter supplier name</t>
+  </si>
+  <si>
+    <t>CustomerTable</t>
+  </si>
+  <si>
+    <t>captureCustomer</t>
+  </si>
+  <si>
+    <t>Adithya</t>
+  </si>
+  <si>
+    <t>Ameerpet plot number 243</t>
+  </si>
+  <si>
+    <t>I am a customer for Goods</t>
+  </si>
+  <si>
+    <t>(//a[contains(.,'Customers')])[2]</t>
+  </si>
+  <si>
+    <t>x_Customer_Number</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Customer_Name']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +496,43 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,10 +587,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -449,8 +619,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +944,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -777,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -789,7 +968,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -801,7 +980,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -813,7 +992,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -1052,7 +1231,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:E20"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2055,18 +2234,624 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="10">
+        <v>10</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="18">
+        <v>10</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="13">
+        <v>10</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="4">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2467891</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="16">
+        <v>9989786487</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="13">
+        <v>10</v>
+      </c>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="13">
+        <v>10</v>
+      </c>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="17"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E23" r:id="rId1" display="test123@gmail.com"/>
+    <hyperlink ref="E22" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2107,6 +2892,7 @@
       <c r="E2" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2124,6 +2910,7 @@
       <c r="E3" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -2141,6 +2928,7 @@
       <c r="E4" s="10">
         <v>10</v>
       </c>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -2158,6 +2946,7 @@
       <c r="E5" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -2175,6 +2964,7 @@
       <c r="E6" s="10" t="s">
         <v>36</v>
       </c>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -2192,6 +2982,7 @@
       <c r="E7" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2209,6 +3000,7 @@
       <c r="E8" s="10">
         <v>10</v>
       </c>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -2226,187 +3018,427 @@
       <c r="E9" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="18">
+        <v>10</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="13">
+        <v>10</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="4">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="4">
+        <v>6991234</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="16">
+        <v>9948016056</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="13">
+        <v>10</v>
+      </c>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="13">
+        <v>10</v>
+      </c>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E23" r:id="rId1" display="test123@gmail.com"/>
+    <hyperlink ref="E22" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>